<commit_message>
Final PCB Layout. Accurate costings
</commit_message>
<xml_diff>
--- a/Documents/Costings.xlsx
+++ b/Documents/Costings.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -42,30 +42,15 @@
     <t>SDRAM</t>
   </si>
   <si>
-    <t>SD Card Connector</t>
-  </si>
-  <si>
-    <t>Serial Data Flash</t>
-  </si>
-  <si>
     <t>I2C Mux</t>
   </si>
   <si>
     <t>OV7670 + Buffer</t>
   </si>
   <si>
-    <t>TFT Screen</t>
-  </si>
-  <si>
-    <t>EEPROM</t>
-  </si>
-  <si>
     <t>Voltage Regulator</t>
   </si>
   <si>
-    <t>Passives</t>
-  </si>
-  <si>
     <t>PCB</t>
   </si>
   <si>
@@ -82,12 +67,42 @@
   </si>
   <si>
     <t>Motor Driver</t>
+  </si>
+  <si>
+    <t>PCB Cart</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Motors</t>
+  </si>
+  <si>
+    <t>GearBox</t>
+  </si>
+  <si>
+    <t>Robot Base</t>
+  </si>
+  <si>
+    <t>Micro SD Card</t>
+  </si>
+  <si>
+    <t>Micro SD Card Connector</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Zepler Stores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,8 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,19 +436,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -460,126 +477,249 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>0.81</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*D3</f>
+        <v>0.81</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*D4</f>
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>2.04</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*D5</f>
+        <v>2.04</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="D6">
         <v>15.39</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3">
-        <v>3.24</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>0.81</v>
-      </c>
       <c r="E6">
         <v>1</v>
       </c>
+      <c r="F6" s="1">
+        <f>E6*D6</f>
+        <v>15.39</v>
+      </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>1.07</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
+      <c r="F7" s="1">
+        <f>E7*D7</f>
+        <v>2.14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>205.48</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*D10</f>
+        <v>205.48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="D12">
+        <v>3.24</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*D12</f>
+        <v>3.24</v>
+      </c>
+      <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>1.03</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
+      <c r="F13" s="1">
+        <f>E13*D13</f>
+        <v>1.03</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="1">
+        <f>SUM(F2:F13)</f>
+        <v>234.13</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="B1:G13">
+    <sortCondition ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Done some writing on PCB development and added figures of circuit and PCB.
</commit_message>
<xml_diff>
--- a/Documents/Costings.xlsx
+++ b/Documents/Costings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -94,6 +94,60 @@
   </si>
   <si>
     <t>Zepler Stores</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>Capactiors</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>Headers</t>
+  </si>
+  <si>
+    <t>TCRT1010</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>LEDs</t>
+  </si>
+  <si>
+    <t>USB Socket</t>
+  </si>
+  <si>
+    <t>Clock</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>MT48LC4M16A2P</t>
+  </si>
+  <si>
+    <t>TB6593FNG</t>
+  </si>
+  <si>
+    <t>Rapid</t>
+  </si>
+  <si>
+    <t>Optosensor</t>
+  </si>
+  <si>
+    <t>OV7670</t>
+  </si>
+  <si>
+    <t>LM1117MP</t>
+  </si>
+  <si>
+    <t>16MHz</t>
+  </si>
+  <si>
+    <t>Part</t>
   </si>
 </sst>
 </file>
@@ -103,10 +157,22 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF555555"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,9 +198,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,13 +793,407 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>0.155</v>
+      </c>
+      <c r="D3">
+        <v>43</v>
+      </c>
+      <c r="E3" s="1">
+        <f>D3*C3</f>
+        <v>6.665</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <v>1.48</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <f>D4*C4</f>
+        <v>1.48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>0.48</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <f>D5*C5</f>
+        <v>0.48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6">
+        <v>0.51</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <f>D6*C6</f>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>0.81</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <f>D7*C7</f>
+        <v>0.81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>0.158</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <f>D8*C8</f>
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <f>D9*C9</f>
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>2.04</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <f>D10*C10</f>
+        <v>2.04</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>15.39</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <f>D11*C11</f>
+        <v>15.39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>1.07</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <f>D12*C12</f>
+        <v>2.14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>0.42</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <f>D13*C13</f>
+        <v>0.84</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>0.94</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <f>D14*C14</f>
+        <v>1.88</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <f>D15*C15</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <v>0.43</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
+        <f>D16*C16</f>
+        <v>0.86</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D17">
+        <v>46</v>
+      </c>
+      <c r="E17" s="1">
+        <f>D17*C17</f>
+        <v>3.036</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>3.24</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <f>D18*C18</f>
+        <v>3.24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19">
+        <v>0.45</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <f>D19*C19</f>
+        <v>0.45</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20">
+        <v>0.84</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <f>D20*C20</f>
+        <v>0.84</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21">
+        <v>1.03</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <f>D21*C21</f>
+        <v>1.03</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A3:G21">
+    <sortCondition ref="A3:A21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>